<commit_message>
added more feature extraction
added more feature extraction
</commit_message>
<xml_diff>
--- a/clean datasets/mergedset4.xlsx
+++ b/clean datasets/mergedset4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SLY\PycharmProjects\offensivedetection\clean datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA583240-4E2A-4E49-9728-C045F173F68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CDB94A-2443-4D25-B8AA-B472A4DEA164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="540" windowWidth="18765" windowHeight="19845" xr2:uid="{8D731DCA-78C4-4CCE-930A-7E60E7D1EE1E}"/>
+    <workbookView xWindow="18435" yWindow="1800" windowWidth="18765" windowHeight="19845" xr2:uid="{8D731DCA-78C4-4CCE-930A-7E60E7D1EE1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,15 +42,9 @@
     <t>N</t>
   </si>
   <si>
-    <t>gago</t>
-  </si>
-  <si>
     <t>maganda</t>
   </si>
   <si>
-    <t>puta</t>
-  </si>
-  <si>
     <t>comments</t>
   </si>
   <si>
@@ -66,10 +60,16 @@
     <t>pogi</t>
   </si>
   <si>
-    <t>matalino</t>
-  </si>
-  <si>
-    <t>masipag</t>
+    <t>gago punyeta</t>
+  </si>
+  <si>
+    <t>puta gago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">masipag magalang </t>
+  </si>
+  <si>
+    <t>matalino mabait</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,15 +475,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -499,7 +499,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -507,7 +507,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>1</v>
@@ -515,7 +515,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>0</v>
@@ -523,7 +523,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>1</v>
@@ -531,7 +531,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>1</v>
@@ -539,7 +539,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
added new 4 new features and SVM algorithm
- added vowel count
- added consonant count
- added space count
- added SVM algorithm
- added balanced and unbalanced splits
</commit_message>
<xml_diff>
--- a/clean datasets/mergedset4.xlsx
+++ b/clean datasets/mergedset4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SLY\PycharmProjects\offensivedetection\clean datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67744AE-32FF-4CAA-A453-AF874379616E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F51F11-8DFE-4A6D-80E5-2DDBC4CD9460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19860" yWindow="990" windowWidth="16710" windowHeight="19845" xr2:uid="{8D731DCA-78C4-4CCE-930A-7E60E7D1EE1E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{8D731DCA-78C4-4CCE-930A-7E60E7D1EE1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Y</t>
   </si>
@@ -45,18 +45,9 @@
     <t>maganda</t>
   </si>
   <si>
-    <t>bobo tarantado</t>
-  </si>
-  <si>
     <t>pogi</t>
   </si>
   <si>
-    <t>gago punyeta</t>
-  </si>
-  <si>
-    <t>puta gago</t>
-  </si>
-  <si>
     <t>matalino mabait</t>
   </si>
   <si>
@@ -70,6 +61,27 @@
   </si>
   <si>
     <t>tae bobo</t>
+  </si>
+  <si>
+    <t>Yan ung sunod na magdadala Ng pandemia sa [NAME]😠😠😠</t>
+  </si>
+  <si>
+    <t>Naawa ako sa bata at sa magulang niya🥺🥺🥺🥺🥺🥺</t>
+  </si>
+  <si>
+    <t>[NAME] bless kuya [NAME] ♥️♥️</t>
+  </si>
+  <si>
+    <t>bobo tarantado 💩</t>
+  </si>
+  <si>
+    <t>gago punyeta 💩</t>
+  </si>
+  <si>
+    <t>Nakakatakot naman ang ginawa ni tatay at dumugo pa ang kamay nya fuck🖕</t>
+  </si>
+  <si>
+    <t>puta fuck gago 💩</t>
   </si>
 </sst>
 </file>
@@ -462,28 +474,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1802407-1453-4A32-96AA-3DFF10D15D24}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="138.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -491,7 +504,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -499,7 +512,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -515,7 +528,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>0</v>
@@ -523,7 +536,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>1</v>
@@ -531,7 +544,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>1</v>
@@ -539,11 +552,41 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>